<commit_message>
Ground / Power Planes weren't saving gerbers... fixed
</commit_message>
<xml_diff>
--- a/Project/FlightController/Project Outputs for FlightController/BOM/Copy of Bill of Materials-FlightController.xlsx
+++ b/Project/FlightController/Project Outputs for FlightController/BOM/Copy of Bill of Materials-FlightController.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awright\Desktop\FlightController\Project\FlightController\Project Outputs for FlightController\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awright\Desktop\Fresh\FlightController\Project\FlightController\Project Outputs for FlightController\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E892ABFD-F52A-4B76-8466-D2400986FA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4106DAB-F052-4216-9B74-1E5BCE4F61C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="4560" windowWidth="28800" windowHeight="15460" xr2:uid="{E732B9D9-BB65-4B44-AA78-6931F5FB0AA9}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11265" xr2:uid="{51781352-5E8A-4EB0-A8C8-98EF27A86E1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of Bill of Materials-Fligh" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="171">
   <si>
     <t>Line #</t>
   </si>
@@ -86,16 +86,34 @@
     <t/>
   </si>
   <si>
-    <t>Capacitor 4.7µF +/-40% 25V 0805</t>
-  </si>
-  <si>
-    <t>Chip Capacitor, 4.7µF +/-40%, 25V, 0805, Thickness 1.45 mm</t>
-  </si>
-  <si>
-    <t>CMP-001-00080-4</t>
-  </si>
-  <si>
-    <t>Up to date</t>
+    <t>Custom item 1</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC0805FR-07100KL</t>
+  </si>
+  <si>
+    <t>Volume Production</t>
+  </si>
+  <si>
+    <t>Arrow Electronics</t>
+  </si>
+  <si>
+    <t>Custom item 2</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>311-1140-1-ND</t>
+  </si>
+  <si>
+    <t>Custom item 3</t>
   </si>
   <si>
     <t>Kyocera AVX</t>
@@ -104,51 +122,12 @@
     <t>08053D475MAT2A</t>
   </si>
   <si>
-    <t>Volume Production</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
     <t>581-08053D475MAT2A</t>
   </si>
   <si>
-    <t>Capacitor 100 nF +/-10% 50 V 0805</t>
-  </si>
-  <si>
-    <t>Chip Capacitor, 100 nF, +/- 10%, 50 V, 0805 (2012 Metric)</t>
-  </si>
-  <si>
-    <t>CMP-001-00018-6</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
-    <t>CC0805KRX7R9BB104</t>
-  </si>
-  <si>
-    <t>Digi-Key</t>
-  </si>
-  <si>
-    <t>311-1140-1-ND</t>
-  </si>
-  <si>
-    <t>Resistor 100k +/-1% 0805 125 mW</t>
-  </si>
-  <si>
-    <t>Chip Resistor, 100 KOhm, +/- 1%, 0.125 W, -55 to 155 degC, 0805 (2012 Metric)</t>
-  </si>
-  <si>
-    <t>CMP-009-00024-5</t>
-  </si>
-  <si>
-    <t>RC0805FR-07100KL</t>
-  </si>
-  <si>
-    <t>311-100KCRCT-ND</t>
-  </si>
-  <si>
     <t>SML-210MTT86</t>
   </si>
   <si>
@@ -158,9 +137,6 @@
     <t>3.3V, 5V, 9V, Status</t>
   </si>
   <si>
-    <t>CMP-08952-000013-1</t>
-  </si>
-  <si>
     <t>Rohm</t>
   </si>
   <si>
@@ -182,9 +158,6 @@
     <t>C0.1uf_1, C0.1uf_2, C0.1uf_5, C0.1uf_6, C0.1uf_7, C0.1uf_8</t>
   </si>
   <si>
-    <t>CMP-2100-03641-2</t>
-  </si>
-  <si>
     <t>Murata</t>
   </si>
   <si>
@@ -200,9 +173,6 @@
     <t>C0.47uf_2</t>
   </si>
   <si>
-    <t>CMP-2006-02860-2</t>
-  </si>
-  <si>
     <t>Newark</t>
   </si>
   <si>
@@ -218,15 +188,9 @@
     <t>C2.2nf, C2.2nf_1</t>
   </si>
   <si>
-    <t>CMP-2006-02908-5</t>
-  </si>
-  <si>
     <t>Obsolete</t>
   </si>
   <si>
-    <t>Arrow Electronics</t>
-  </si>
-  <si>
     <t>GRM188R60J106ME47D</t>
   </si>
   <si>
@@ -236,9 +200,6 @@
     <t>C10u_1, C10uf_2, C10uf_3, C10uf_4</t>
   </si>
   <si>
-    <t>CMP-2006-02792-2</t>
-  </si>
-  <si>
     <t>03AC2652</t>
   </si>
   <si>
@@ -251,9 +212,6 @@
     <t>C22_uf_2, C22uf_4</t>
   </si>
   <si>
-    <t>CMP-2007-03385-2</t>
-  </si>
-  <si>
     <t>24R6338</t>
   </si>
   <si>
@@ -266,9 +224,6 @@
     <t>C100nf, C100nf_1, C100nf_2, C100nf_3, C100nf_4, C100nf_5, C100nf_6, C100nf_7, C100nf_B1, C100nf_B2</t>
   </si>
   <si>
-    <t>CMP-2008-02046-2</t>
-  </si>
-  <si>
     <t>KEMET</t>
   </si>
   <si>
@@ -284,9 +239,6 @@
     <t>C100uf_3, C100uf_4</t>
   </si>
   <si>
-    <t>CMP-2000-05259-2</t>
-  </si>
-  <si>
     <t>2114105</t>
   </si>
   <si>
@@ -299,18 +251,12 @@
     <t>CD1</t>
   </si>
   <si>
-    <t>CMP-2000-05248-1</t>
-  </si>
-  <si>
     <t>Molex</t>
   </si>
   <si>
     <t>5027740891</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>67X4867</t>
   </si>
   <si>
@@ -323,9 +269,6 @@
     <t>D?</t>
   </si>
   <si>
-    <t>CMP-14398-000007-1</t>
-  </si>
-  <si>
     <t>Nexperia</t>
   </si>
   <si>
@@ -341,9 +284,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>CMP-2000-05827-1</t>
-  </si>
-  <si>
     <t>1050170001</t>
   </si>
   <si>
@@ -359,9 +299,6 @@
     <t>J2</t>
   </si>
   <si>
-    <t>CMP-205963-000001-1</t>
-  </si>
-  <si>
     <t>Tag-Connect</t>
   </si>
   <si>
@@ -374,9 +311,6 @@
     <t>P1</t>
   </si>
   <si>
-    <t>CMP-2000-07082-1</t>
-  </si>
-  <si>
     <t>JST</t>
   </si>
   <si>
@@ -392,9 +326,6 @@
     <t>P2, P3</t>
   </si>
   <si>
-    <t>CMP-2000-07080-1</t>
-  </si>
-  <si>
     <t>455-1806-1-ND</t>
   </si>
   <si>
@@ -407,9 +338,6 @@
     <t>P5</t>
   </si>
   <si>
-    <t>CMP-2000-07077-1</t>
-  </si>
-  <si>
     <t>33P8180</t>
   </si>
   <si>
@@ -422,9 +350,6 @@
     <t>R1K_1, R1K_2, R1K_3, R4_LED, R5_LED</t>
   </si>
   <si>
-    <t>CMP-1666-00003-5</t>
-  </si>
-  <si>
     <t>Vishay Dale</t>
   </si>
   <si>
@@ -437,9 +362,6 @@
     <t>R2.2K_1, R2.2K_2</t>
   </si>
   <si>
-    <t>CMP-2000-03167-1</t>
-  </si>
-  <si>
     <t>Vishay</t>
   </si>
   <si>
@@ -452,18 +374,12 @@
     <t>R4.7K_1</t>
   </si>
   <si>
-    <t>CMP-2002-00051-3</t>
-  </si>
-  <si>
     <t>CRCW06032K00FKEA</t>
   </si>
   <si>
     <t>R6_LED, R7_LED, R8_LED</t>
   </si>
   <si>
-    <t>CMP-2000-03159-1</t>
-  </si>
-  <si>
     <t>52K8224</t>
   </si>
   <si>
@@ -476,9 +392,6 @@
     <t>R10K_1, R10K_2, R10K_3, R10K_4</t>
   </si>
   <si>
-    <t>CMP-1666-00005-4</t>
-  </si>
-  <si>
     <t>52K8063</t>
   </si>
   <si>
@@ -488,9 +401,6 @@
     <t>R22_1, R22_2</t>
   </si>
   <si>
-    <t>CMP-2002-08382-1</t>
-  </si>
-  <si>
     <t>52K6848</t>
   </si>
   <si>
@@ -500,9 +410,6 @@
     <t>R75_1, R75_2</t>
   </si>
   <si>
-    <t>CMP-2000-00639-1</t>
-  </si>
-  <si>
     <t>Panasonic</t>
   </si>
   <si>
@@ -518,9 +425,6 @@
     <t>R150_1</t>
   </si>
   <si>
-    <t>CMP-2000-03913-2</t>
-  </si>
-  <si>
     <t>52K8161</t>
   </si>
   <si>
@@ -533,9 +437,6 @@
     <t>SW1</t>
   </si>
   <si>
-    <t>CMP-08834-000005-1</t>
-  </si>
-  <si>
     <t>Omron</t>
   </si>
   <si>
@@ -551,9 +452,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>CMP-12105-000139-1</t>
-  </si>
-  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
@@ -566,9 +464,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>CMP-2000-05008-1</t>
-  </si>
-  <si>
     <t>TDK InvenSense</t>
   </si>
   <si>
@@ -581,9 +476,6 @@
     <t>U3</t>
   </si>
   <si>
-    <t>CMP-2000-05076-3</t>
-  </si>
-  <si>
     <t>Bosch</t>
   </si>
   <si>
@@ -599,9 +491,6 @@
     <t>U5</t>
   </si>
   <si>
-    <t>CMP-2000-07341-2</t>
-  </si>
-  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
@@ -617,9 +506,6 @@
     <t>U6</t>
   </si>
   <si>
-    <t>CMP-0244-00310-1</t>
-  </si>
-  <si>
     <t>511-LD1117S33</t>
   </si>
   <si>
@@ -632,9 +518,6 @@
     <t>U8</t>
   </si>
   <si>
-    <t>CMP-05676-000004-1</t>
-  </si>
-  <si>
     <t>Maxim</t>
   </si>
   <si>
@@ -647,9 +530,6 @@
     <t>U9</t>
   </si>
   <si>
-    <t>CMP-04917-000367-1</t>
-  </si>
-  <si>
     <t>595-TLV76790QWDRBRQ1</t>
   </si>
   <si>
@@ -662,9 +542,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>CMP-2100-03620-1</t>
-  </si>
-  <si>
     <t>ABM3-27.000MHZ-D2Y-T</t>
   </si>
   <si>
@@ -672,9 +549,6 @@
   </si>
   <si>
     <t>Y2</t>
-  </si>
-  <si>
-    <t>CMP-27762-013610-1</t>
   </si>
   <si>
     <t>Abracon</t>
@@ -1053,7 +927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846ACF55-C83D-464C-8032-6ADD17659236}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380FD84B-DE29-4E20-A189-3072E65E750F}">
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1126,34 +1000,30 @@
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1">
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -1167,37 +1037,33 @@
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
@@ -1211,37 +1077,33 @@
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="L4" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="M4" s="1">
         <v>0</v>
@@ -1255,37 +1117,33 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1">
         <v>4</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="M5" s="1">
         <v>0.34</v>
@@ -1299,37 +1157,33 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1">
         <v>6</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="M6" s="1">
         <v>1.7000000000000001E-2</v>
@@ -1343,37 +1197,33 @@
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="M7" s="1">
         <v>2.1000000000000001E-2</v>
@@ -1387,37 +1237,33 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1">
         <v>2</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="M8" s="1">
         <v>1.38E-2</v>
@@ -1431,37 +1277,33 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1">
         <v>4</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="M9" s="1">
         <v>2.9000000000000001E-2</v>
@@ -1475,37 +1317,33 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1">
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="M10" s="1">
         <v>7.6999999999999999E-2</v>
@@ -1519,37 +1357,33 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="1">
         <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="M11" s="1">
         <v>5.0000000000000001E-3</v>
@@ -1563,37 +1397,33 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="1">
         <v>2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="M12" s="1">
         <v>1.23</v>
@@ -1607,37 +1437,33 @@
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
       <c r="G13" s="1">
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="M13" s="1">
         <v>2.58</v>
@@ -1651,37 +1477,33 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="1">
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="M14" s="1">
         <v>3.5999999999999997E-2</v>
@@ -1695,37 +1517,33 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1">
         <v>1</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="M15" s="1">
         <v>0.23499999999999999</v>
@@ -1735,33 +1553,31 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="1">
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1773,37 +1589,33 @@
         <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="1">
         <v>1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="M17" s="1">
         <v>0.88</v>
@@ -1817,37 +1629,33 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="1">
         <v>2</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="M18" s="1">
         <v>0.78</v>
@@ -1861,37 +1669,33 @@
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="1">
         <v>1</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="M19" s="1">
         <v>0.54</v>
@@ -1905,37 +1709,33 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" s="1">
         <v>5</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="M20" s="1">
         <v>5.0000000000000001E-3</v>
@@ -1949,37 +1749,33 @@
         <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
       <c r="G21" s="1">
         <v>2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="M21" s="1">
         <v>2.4799999999999999E-2</v>
@@ -1993,31 +1789,27 @@
         <v>14</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
       <c r="G22" s="1">
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2029,37 +1821,33 @@
         <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
       <c r="G23" s="1">
         <v>3</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="M23" s="1">
         <v>6.0000000000000001E-3</v>
@@ -2073,37 +1861,33 @@
         <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
       <c r="G24" s="1">
         <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="M24" s="1">
         <v>5.0000000000000001E-3</v>
@@ -2117,37 +1901,33 @@
         <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
       <c r="G25" s="1">
         <v>2</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="M25" s="1">
         <v>3.0000000000000001E-3</v>
@@ -2161,37 +1941,33 @@
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="1">
         <v>2</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="M26" s="1">
         <v>3.0000000000000001E-3</v>
@@ -2205,37 +1981,33 @@
         <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
       <c r="G27" s="1">
         <v>1</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="M27" s="1">
         <v>5.0000000000000001E-3</v>
@@ -2249,37 +2021,33 @@
         <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
       <c r="G28" s="1">
         <v>1</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="M28" s="1">
         <v>1.01</v>
@@ -2293,31 +2061,27 @@
         <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
       <c r="G29" s="1">
         <v>1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -2329,31 +2093,27 @@
         <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="1">
         <v>1</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -2365,31 +2125,27 @@
         <v>14</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
       <c r="G31" s="1">
         <v>1</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -2401,37 +2157,33 @@
         <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
       <c r="G32" s="1">
         <v>1</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="M32" s="1">
         <v>0.49</v>
@@ -2445,37 +2197,33 @@
         <v>14</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="G33" s="1">
         <v>1</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="M33" s="1">
         <v>0.66</v>
@@ -2489,31 +2237,27 @@
         <v>14</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
       <c r="G34" s="1">
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -2525,37 +2269,33 @@
         <v>14</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="G35" s="1">
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="M35" s="1">
         <v>1.49</v>
@@ -2569,31 +2309,27 @@
         <v>14</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
       <c r="G36" s="1">
         <v>1</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -2605,37 +2341,33 @@
         <v>14</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>209</v>
+        <v>168</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
       <c r="G37" s="1">
         <v>1</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>212</v>
+        <v>170</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="M37" s="1">
         <v>0.40770000000000001</v>

</xml_diff>

<commit_message>
Think this version may actually get made, time will tell
</commit_message>
<xml_diff>
--- a/Project/FlightController/Project Outputs for FlightController/BOM/Copy of Bill of Materials-FlightController.xlsx
+++ b/Project/FlightController/Project Outputs for FlightController/BOM/Copy of Bill of Materials-FlightController.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awright\Desktop\FlightController\Project\FlightController\Project Outputs for FlightController\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{188CB882-B16F-44ED-9C59-8ED382EA2AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3D71974-CB5D-4834-936C-CA7B74A724DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="4940" windowWidth="28800" windowHeight="15460" xr2:uid="{A6A766C7-FA90-4824-AC1C-2D5C2C028DCB}"/>
+    <workbookView xWindow="5280" yWindow="5280" windowWidth="28800" windowHeight="15460" xr2:uid="{ED931E05-E3B8-4D7A-91D6-3F786FA359E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of Bill of Materials-Fligh" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
     <t>RC0805FR-07100KL</t>
   </si>
   <si>
-    <t>311-100KCRCT-ND</t>
+    <t>311-100KCRDKR-ND</t>
   </si>
   <si>
     <t>SML-210MTT86</t>
@@ -1152,7 +1152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6AF20A-5B38-4D24-9ABF-267FD75967CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B7E6C0-B85B-45C2-9F26-45737331CD95}">
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1164,7 +1164,8 @@
     <col min="3" max="4" width="12.6328125" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="8" width="15.81640625" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="26.453125" customWidth="1"/>
     <col min="11" max="11" width="22.90625" customWidth="1"/>

</xml_diff>

<commit_message>
Add load caps to the 27mhz crystal
</commit_message>
<xml_diff>
--- a/Project/FlightController/Project Outputs for FlightController/BOM/Copy of Bill of Materials-FlightController.xlsx
+++ b/Project/FlightController/Project Outputs for FlightController/BOM/Copy of Bill of Materials-FlightController.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awright\Desktop\FlightController\Project\FlightController\Project Outputs for FlightController\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3D71974-CB5D-4834-936C-CA7B74A724DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1361BFB-7016-4876-9CF8-EAD3AF1AE14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="5280" windowWidth="28800" windowHeight="15460" xr2:uid="{ED931E05-E3B8-4D7A-91D6-3F786FA359E5}"/>
+    <workbookView xWindow="5280" yWindow="5280" windowWidth="28800" windowHeight="15460" xr2:uid="{9387BB20-26BD-4E6C-A6EC-DF58FBB67DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of Bill of Materials-Fligh" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="234">
   <si>
     <t>Name</t>
   </si>
@@ -86,397 +86,361 @@
     <t>Supplier Subtotal 1</t>
   </si>
   <si>
-    <t>Capacitor 4.7µF +/-40% 25V 0805</t>
-  </si>
-  <si>
-    <t>Chip Capacitor, 4.7µF +/-40%, 25V, 0805, Thickness 1.45 mm</t>
+    <t>SML-210MTT86</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>3.3V, 5V, 9V, Status</t>
+  </si>
+  <si>
+    <t>CMP-08952-000013-1</t>
+  </si>
+  <si>
+    <t>Up to date</t>
+  </si>
+  <si>
+    <t>FP-SML-210-MFG</t>
+  </si>
+  <si>
+    <t>Rohm</t>
+  </si>
+  <si>
+    <t>Not Recommended for New Design</t>
+  </si>
+  <si>
+    <t>Future Electronics</t>
+  </si>
+  <si>
+    <t>9239369</t>
+  </si>
+  <si>
+    <t>GRM155R71C104KA88D</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t>C0.1uf_1, C0.1uf_2, C0.1uf_5, C0.1uf_6, C0.1uf_7, C0.1uf_8</t>
+  </si>
+  <si>
+    <t>CMP-2100-03641-2</t>
+  </si>
+  <si>
+    <t>FP-GRM15-MFG</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>81-GRM155R71C104KA88</t>
+  </si>
+  <si>
+    <t>GRM188R71C474KA88D</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0603, 0.47uF, X7R, 15%, 10%, 16V</t>
+  </si>
+  <si>
+    <t>C0.47uf_2</t>
+  </si>
+  <si>
+    <t>CMP-2006-02860-2</t>
+  </si>
+  <si>
+    <t>FP-GRM188-0_1-e0_2_0_5-IPC_B</t>
+  </si>
+  <si>
+    <t>Volume Production</t>
+  </si>
+  <si>
+    <t>Newark</t>
+  </si>
+  <si>
+    <t>03AC2674</t>
+  </si>
+  <si>
+    <t>GRM188R71H222KA01D</t>
+  </si>
+  <si>
+    <t>Chip Capacitor, 2.2 nF, +/- 10%, 50 V, -55 to 125 degC, 0603 (1608 Metric), RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>C2.2nf, C2.2nf_1</t>
+  </si>
+  <si>
+    <t>CMP-2006-02908-5</t>
+  </si>
+  <si>
+    <t>CAPC1608X90X35NL10T15</t>
+  </si>
+  <si>
+    <t>Obsolete</t>
+  </si>
+  <si>
+    <t>Arrow Electronics</t>
+  </si>
+  <si>
+    <t>GRM188R60J106ME47D</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0603, 10uF, X5R, 15%, 20%, 6.3V</t>
+  </si>
+  <si>
+    <t>C10u_1, C10uf_2, C10uf_3, C10uf_4</t>
+  </si>
+  <si>
+    <t>CMP-2006-02792-2</t>
+  </si>
+  <si>
+    <t>FP-GRM188-0_1-e0_2_0_55-IPC_A</t>
+  </si>
+  <si>
+    <t>03AC2652</t>
+  </si>
+  <si>
+    <t>C0805C180J5GACTU</t>
+  </si>
+  <si>
+    <t>CAP CER 18PF 50V C0G/NP0 0805</t>
+  </si>
+  <si>
+    <t>C18pf_1, CC18pf_2</t>
+  </si>
+  <si>
+    <t>CMP-2007-00302-2</t>
+  </si>
+  <si>
+    <t>FP-C0805C-DN-MFG</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>GRM21BR60J226ME39L</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0805, 22uF, X5R, 15%, 20%, 6.3V</t>
+  </si>
+  <si>
+    <t>C22_uf_2, C22uf_4</t>
+  </si>
+  <si>
+    <t>CMP-2007-03385-2</t>
+  </si>
+  <si>
+    <t>FP-GRM21B-0_15-MFG</t>
+  </si>
+  <si>
+    <t>24R6338</t>
+  </si>
+  <si>
+    <t>C0402C104K8PACTU</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 10V X5R 0402</t>
+  </si>
+  <si>
+    <t>C100nf, C100nf_1, C100nf_2, C100nf_3, C100nf_4, C100nf_5, C100nf_6, C100nf_7, C100nf_B1, C100nf_B2</t>
+  </si>
+  <si>
+    <t>CMP-2008-02046-2</t>
+  </si>
+  <si>
+    <t>FP-C0402-BB-MFG</t>
+  </si>
+  <si>
+    <t>49H5566</t>
+  </si>
+  <si>
+    <t>GRM32ER60J107ME20L</t>
+  </si>
+  <si>
+    <t>CAP CER 100UF 6.3V X5R 1210</t>
+  </si>
+  <si>
+    <t>C100uf_3, C100uf_4</t>
+  </si>
+  <si>
+    <t>CMP-2000-05259-2</t>
+  </si>
+  <si>
+    <t>FP-GRM32-0_3-MFG</t>
+  </si>
+  <si>
+    <t>2114105</t>
+  </si>
+  <si>
+    <t>502774-0891</t>
+  </si>
+  <si>
+    <t>Micro SD Memory Card Connector, 0.5 A, 10 V (DC), -25 to 85 degC, 8-Pin SMT, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>CD1</t>
+  </si>
+  <si>
+    <t>CMP-2000-05248-1</t>
+  </si>
+  <si>
+    <t>MOLX-502774-0891_V</t>
+  </si>
+  <si>
+    <t>https://datasheet.ciiva.com/1104/1499551-1104671.pdf</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>5027740891</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>67X4867</t>
+  </si>
+  <si>
+    <t>BAT54C,215</t>
+  </si>
+  <si>
+    <t>DIODE ARRAY SCHOTTKY 30V SOT23</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>CMP-14398-000007-1</t>
+  </si>
+  <si>
+    <t>FP-SOT23-MFG</t>
+  </si>
+  <si>
+    <t>Nexperia</t>
+  </si>
+  <si>
+    <t>97W1832</t>
+  </si>
+  <si>
+    <t>105017-0001</t>
+  </si>
+  <si>
+    <t>Micro-USB B Receptacle, Right Angle, Bottom Mount, Surface Mount, with Solder Tabs, -30 to 85 degC, 5-Pin USB, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>CMP-2000-05827-1</t>
+  </si>
+  <si>
+    <t>USB-MICRO-B_V</t>
+  </si>
+  <si>
+    <t>http://www.molex.com/elqNow/elqRedir.htm?ref=http://www.molex.com/webdocs/datasheets/pdf/en-us/1050170001_IO_CONNECTORS.pdf</t>
+  </si>
+  <si>
+    <t>1050170001</t>
+  </si>
+  <si>
+    <t>17AC5641</t>
+  </si>
+  <si>
+    <t>SM08B-SRSS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>Male Header, Pitch 1 mm, 1 x 8 Position, Height 2.95 mm, -25 to 85 degC, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>CMP-2000-07082-1</t>
+  </si>
+  <si>
+    <t>JST-SM08B-SRSS-TB_V</t>
+  </si>
+  <si>
+    <t>http://www.jst-mfg.com/product/pdf/eng/eSR.pdf</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>455-1808-1-ND</t>
+  </si>
+  <si>
+    <t>SM06B-SRSS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>Male Header, Pitch 1 mm, 1 x 6 Position, Height 2.95 mm, -25 to 85 degC, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>P2, P3</t>
+  </si>
+  <si>
+    <t>CMP-2000-07080-1</t>
+  </si>
+  <si>
+    <t>JST-SM06B-SRSS-TB_V</t>
+  </si>
+  <si>
+    <t>https://datasheet.ciiva.com/26894/getdatasheetpartid-708885-26894671.pdf</t>
+  </si>
+  <si>
+    <t>455-1806-1-ND</t>
+  </si>
+  <si>
+    <t>SM03B-SRSS-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>Male Header, Pitch 1 mm, 1 x 3 Position, Height 2.9 mm, -25 to 85 degC, RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>CMP-2000-07077-1</t>
+  </si>
+  <si>
+    <t>JST-SM03B-SRSS-TB_V</t>
+  </si>
+  <si>
+    <t>33P8180</t>
+  </si>
+  <si>
+    <t>CRCW06031K00FKEA</t>
+  </si>
+  <si>
+    <t>RES Thick Film, 1kΩ, 1%, 0.1W, 100ppm/°C, 0603</t>
+  </si>
+  <si>
+    <t>R1K_1, R1K_2, R1K_3, R4_LED, R5_LED</t>
+  </si>
+  <si>
+    <t>CMP-1666-00003-5</t>
+  </si>
+  <si>
+    <t>FP-CRCW0603-e3-MFG</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>52K8016</t>
+  </si>
+  <si>
+    <t>CRCW06032K20FKEA</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>CMP-001-00080-4</t>
-  </si>
-  <si>
-    <t>Up to date</t>
-  </si>
-  <si>
-    <t>Kyocera AVX</t>
-  </si>
-  <si>
-    <t>08053D475MAT2A</t>
-  </si>
-  <si>
-    <t>Volume Production</t>
-  </si>
-  <si>
-    <t>Mouser</t>
-  </si>
-  <si>
-    <t>581-08053D475MAT2A</t>
-  </si>
-  <si>
-    <t>Capacitor 100 nF +/-10% 50 V 0805</t>
-  </si>
-  <si>
-    <t>Chip Capacitor, 100 nF, +/- 10%, 50 V, 0805 (2012 Metric)</t>
-  </si>
-  <si>
-    <t>CMP-001-00018-6</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
-    <t>CC0805KRX7R9BB104</t>
-  </si>
-  <si>
-    <t>Digi-Key</t>
-  </si>
-  <si>
-    <t>311-1140-1-ND</t>
-  </si>
-  <si>
-    <t>Resistor 100k +/-1% 0805 125 mW</t>
-  </si>
-  <si>
-    <t>Chip Resistor, 100 KOhm, +/- 1%, 0.125 W, -55 to 155 degC, 0805 (2012 Metric)</t>
-  </si>
-  <si>
-    <t>CMP-009-00024-5</t>
-  </si>
-  <si>
-    <t>RC0805FR-07100KL</t>
-  </si>
-  <si>
-    <t>311-100KCRDKR-ND</t>
-  </si>
-  <si>
-    <t>SML-210MTT86</t>
-  </si>
-  <si>
-    <t>LED GREEN CLEAR 0805 SMD</t>
-  </si>
-  <si>
-    <t>3.3V, 5V, 9V, Status</t>
-  </si>
-  <si>
-    <t>CMP-08952-000013-1</t>
-  </si>
-  <si>
-    <t>FP-SML-210-MFG</t>
-  </si>
-  <si>
-    <t>Rohm</t>
-  </si>
-  <si>
-    <t>Not Recommended for New Design</t>
-  </si>
-  <si>
-    <t>Future Electronics</t>
-  </si>
-  <si>
-    <t>9239369</t>
-  </si>
-  <si>
-    <t>GRM155R71C104KA88D</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 16V X7R 0402</t>
-  </si>
-  <si>
-    <t>C0.1uf_1, C0.1uf_2, C0.1uf_5, C0.1uf_6, C0.1uf_7, C0.1uf_8</t>
-  </si>
-  <si>
-    <t>CMP-2100-03641-2</t>
-  </si>
-  <si>
-    <t>FP-GRM15-MFG</t>
-  </si>
-  <si>
-    <t>Murata</t>
-  </si>
-  <si>
-    <t>81-GRM155R71C104KA88</t>
-  </si>
-  <si>
-    <t>GRM188R71C474KA88D</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0603, 0.47uF, X7R, 15%, 10%, 16V</t>
-  </si>
-  <si>
-    <t>C0.47uf_2</t>
-  </si>
-  <si>
-    <t>CMP-2006-02860-2</t>
-  </si>
-  <si>
-    <t>FP-GRM188-0_1-e0_2_0_5-IPC_B</t>
-  </si>
-  <si>
-    <t>Newark</t>
-  </si>
-  <si>
-    <t>03AC2674</t>
-  </si>
-  <si>
-    <t>GRM188R71H222KA01D</t>
-  </si>
-  <si>
-    <t>Chip Capacitor, 2.2 nF, +/- 10%, 50 V, -55 to 125 degC, 0603 (1608 Metric), RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>C2.2nf, C2.2nf_1</t>
-  </si>
-  <si>
-    <t>CMP-2006-02908-5</t>
-  </si>
-  <si>
-    <t>CAPC1608X90X35NL10T15</t>
-  </si>
-  <si>
-    <t>Obsolete</t>
-  </si>
-  <si>
-    <t>Arrow Electronics</t>
-  </si>
-  <si>
-    <t>GRM188R60J106ME47D</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0603, 10uF, X5R, 15%, 20%, 6.3V</t>
-  </si>
-  <si>
-    <t>C10u_1, C10uf_2, C10uf_3, C10uf_4</t>
-  </si>
-  <si>
-    <t>CMP-2006-02792-2</t>
-  </si>
-  <si>
-    <t>FP-GRM188-0_1-e0_2_0_55-IPC_A</t>
-  </si>
-  <si>
-    <t>03AC2652</t>
-  </si>
-  <si>
-    <t>GRM21BR60J226ME39L</t>
-  </si>
-  <si>
-    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0805, 22uF, X5R, 15%, 20%, 6.3V</t>
-  </si>
-  <si>
-    <t>C22_uf_2, C22uf_4</t>
-  </si>
-  <si>
-    <t>CMP-2007-03385-2</t>
-  </si>
-  <si>
-    <t>FP-GRM21B-0_15-MFG</t>
-  </si>
-  <si>
-    <t>24R6338</t>
-  </si>
-  <si>
-    <t>C0402C104K8PACTU</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 10V X5R 0402</t>
-  </si>
-  <si>
-    <t>C100nf, C100nf_1, C100nf_2, C100nf_3, C100nf_4, C100nf_5, C100nf_6, C100nf_7, C100nf_B1, C100nf_B2</t>
-  </si>
-  <si>
-    <t>CMP-2008-02046-2</t>
-  </si>
-  <si>
-    <t>FP-C0402-BB-MFG</t>
-  </si>
-  <si>
-    <t>KEMET</t>
-  </si>
-  <si>
-    <t>49H5566</t>
-  </si>
-  <si>
-    <t>GRM32ER60J107ME20L</t>
-  </si>
-  <si>
-    <t>CAP CER 100UF 6.3V X5R 1210</t>
-  </si>
-  <si>
-    <t>C100uf_3, C100uf_4</t>
-  </si>
-  <si>
-    <t>CMP-2000-05259-2</t>
-  </si>
-  <si>
-    <t>FP-GRM32-0_3-MFG</t>
-  </si>
-  <si>
-    <t>2114105</t>
-  </si>
-  <si>
-    <t>502774-0891</t>
-  </si>
-  <si>
-    <t>Micro SD Memory Card Connector, 0.5 A, 10 V (DC), -25 to 85 degC, 8-Pin SMT, RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>CD1</t>
-  </si>
-  <si>
-    <t>CMP-2000-05248-1</t>
-  </si>
-  <si>
-    <t>MOLX-502774-0891_V</t>
-  </si>
-  <si>
-    <t>https://datasheet.ciiva.com/1104/1499551-1104671.pdf</t>
-  </si>
-  <si>
-    <t>Molex</t>
-  </si>
-  <si>
-    <t>5027740891</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>67X4867</t>
-  </si>
-  <si>
-    <t>BAT54C,215</t>
-  </si>
-  <si>
-    <t>DIODE ARRAY SCHOTTKY 30V SOT23</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>CMP-14398-000007-1</t>
-  </si>
-  <si>
-    <t>FP-SOT23-MFG</t>
-  </si>
-  <si>
-    <t>Nexperia</t>
-  </si>
-  <si>
-    <t>97W1832</t>
-  </si>
-  <si>
-    <t>105017-0001</t>
-  </si>
-  <si>
-    <t>Micro-USB B Receptacle, Right Angle, Bottom Mount, Surface Mount, with Solder Tabs, -30 to 85 degC, 5-Pin USB, RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>CMP-2000-05827-1</t>
-  </si>
-  <si>
-    <t>USB-MICRO-B_V</t>
-  </si>
-  <si>
-    <t>http://www.molex.com/elqNow/elqRedir.htm?ref=http://www.molex.com/webdocs/datasheets/pdf/en-us/1050170001_IO_CONNECTORS.pdf</t>
-  </si>
-  <si>
-    <t>1050170001</t>
-  </si>
-  <si>
-    <t>17AC5641</t>
-  </si>
-  <si>
-    <t>SM08B-SRSS-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>Male Header, Pitch 1 mm, 1 x 8 Position, Height 2.95 mm, -25 to 85 degC, RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>CMP-2000-07082-1</t>
-  </si>
-  <si>
-    <t>JST-SM08B-SRSS-TB_V</t>
-  </si>
-  <si>
-    <t>http://www.jst-mfg.com/product/pdf/eng/eSR.pdf</t>
-  </si>
-  <si>
-    <t>JST</t>
-  </si>
-  <si>
-    <t>455-1808-1-ND</t>
-  </si>
-  <si>
-    <t>SM06B-SRSS-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>Male Header, Pitch 1 mm, 1 x 6 Position, Height 2.95 mm, -25 to 85 degC, RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>P2, P3</t>
-  </si>
-  <si>
-    <t>CMP-2000-07080-1</t>
-  </si>
-  <si>
-    <t>JST-SM06B-SRSS-TB_V</t>
-  </si>
-  <si>
-    <t>https://datasheet.ciiva.com/26894/getdatasheetpartid-708885-26894671.pdf</t>
-  </si>
-  <si>
-    <t>455-1806-1-ND</t>
-  </si>
-  <si>
-    <t>SM03B-SRSS-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>Male Header, Pitch 1 mm, 1 x 3 Position, Height 2.9 mm, -25 to 85 degC, RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>CMP-2000-07077-1</t>
-  </si>
-  <si>
-    <t>JST-SM03B-SRSS-TB_V</t>
-  </si>
-  <si>
-    <t>33P8180</t>
-  </si>
-  <si>
-    <t>CRCW06031K00FKEA</t>
-  </si>
-  <si>
-    <t>RES Thick Film, 1kΩ, 1%, 0.1W, 100ppm/°C, 0603</t>
-  </si>
-  <si>
-    <t>R1K_1, R1K_2, R1K_3, R4_LED, R5_LED</t>
-  </si>
-  <si>
-    <t>CMP-1666-00003-5</t>
-  </si>
-  <si>
-    <t>FP-CRCW0603-e3-MFG</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>52K8016</t>
-  </si>
-  <si>
-    <t>CRCW06032K20FKEA</t>
   </si>
   <si>
     <t>R2.2K_1, R2.2K_2</t>
@@ -1152,8 +1116,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B7E6C0-B85B-45C2-9F26-45737331CD95}">
-  <dimension ref="A1:O36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897C6EAF-9031-4D77-90F3-A1BF237735A7}">
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1239,15 +1203,17 @@
         <v>19</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>22</v>
@@ -1259,10 +1225,10 @@
         <v>24</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -1273,218 +1239,214 @@
         <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N3" s="1">
-        <v>0</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="O3" s="1">
-        <v>0</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="N5" s="1">
-        <v>0.34</v>
+        <v>1.3899999999999999E-2</v>
       </c>
       <c r="O5" s="1">
-        <v>1.36</v>
+        <v>55.6</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N6" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="O6" s="1">
-        <v>0.17</v>
+        <v>0.11600000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" s="1">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="O7" s="1">
-        <v>2.1000000000000001E-2</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -1510,84 +1472,84 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>60</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="N8" s="1">
-        <v>1.3899999999999999E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="O8" s="1">
-        <v>55.6</v>
+        <v>0.154</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="1">
-        <v>4</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N9" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O9" s="1">
-        <v>0.11600000000000001</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>
@@ -1596,133 +1558,135 @@
         <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N10" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>1.23</v>
       </c>
       <c r="O10" s="1">
-        <v>0.154</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="1">
-        <v>10</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="1"/>
       <c r="I11" s="2" t="s">
         <v>84</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="N11" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>2.58</v>
       </c>
       <c r="O11" s="1">
-        <v>0.05</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="2" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="N12" s="1">
-        <v>1.23</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="O12" s="1">
-        <v>2.46</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>19</v>
@@ -1731,45 +1695,45 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N13" s="1">
-        <v>2.58</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="O13" s="1">
-        <v>2.58</v>
+        <v>0.23499999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>19</v>
@@ -1778,90 +1742,92 @@
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="I14" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="N14" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>0.88</v>
       </c>
       <c r="O14" s="1">
-        <v>3.5999999999999997E-2</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="J15" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="M15" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="N15" s="1">
-        <v>0.23499999999999999</v>
+        <v>0.78</v>
       </c>
       <c r="O15" s="1">
-        <v>0.23499999999999999</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>19</v>
@@ -1870,31 +1836,31 @@
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>124</v>
       </c>
       <c r="N16" s="1">
-        <v>0.88</v>
+        <v>0.54</v>
       </c>
       <c r="O16" s="1">
-        <v>0.88</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -1914,34 +1880,32 @@
         <v>19</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="1"/>
+      <c r="I17" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>125</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>131</v>
       </c>
       <c r="N17" s="1">
-        <v>0.78</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O17" s="1">
-        <v>1.56</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
@@ -1961,34 +1925,32 @@
         <v>19</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="H18" s="1"/>
       <c r="I18" s="2" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>132</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="N18" s="1">
-        <v>0.54</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="O18" s="1">
-        <v>0.54</v>
+        <v>4.9599999999999998E-2</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
@@ -2008,212 +1970,212 @@
         <v>19</v>
       </c>
       <c r="F19" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>142</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>138</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="N19" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="O19" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="N20" s="1">
-        <v>2.4799999999999999E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="O20" s="1">
-        <v>4.9599999999999998E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="N21" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="1">
-        <v>3</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N22" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O22" s="1">
         <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="O22" s="1">
-        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="1">
-        <v>4</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="2" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N23" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="O23" s="1">
-        <v>0.02</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>167</v>
@@ -2225,40 +2187,40 @@
         <v>19</v>
       </c>
       <c r="F24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N24" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O24" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>172</v>
@@ -2270,7 +2232,7 @@
         <v>19</v>
       </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>174</v>
@@ -2280,22 +2242,22 @@
         <v>175</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>176</v>
       </c>
       <c r="N25" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>0.66</v>
       </c>
       <c r="O25" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
@@ -2318,43 +2280,35 @@
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="2" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>177</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="N26" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="O26" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>19</v>
@@ -2363,43 +2317,37 @@
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="H27" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="I27" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="N27" s="1">
-        <v>0.66</v>
-      </c>
-      <c r="O27" s="1">
-        <v>0.66</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>19</v>
@@ -2408,17 +2356,17 @@
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>22</v>
+        <v>196</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2427,16 +2375,16 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>19</v>
@@ -2445,37 +2393,43 @@
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>200</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="H29" s="1"/>
       <c r="I29" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0.51</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>19</v>
@@ -2484,35 +2438,43 @@
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="2" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0.307</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0.307</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>19</v>
@@ -2521,30 +2483,22 @@
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="N31" s="1">
-        <v>0.51</v>
-      </c>
-      <c r="O31" s="1">
-        <v>0.51</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
@@ -2570,25 +2524,25 @@
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="2" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>216</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>221</v>
       </c>
       <c r="N32" s="1">
-        <v>0.307</v>
+        <v>1.49</v>
       </c>
       <c r="O32" s="1">
-        <v>0.307</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
@@ -2613,15 +2567,17 @@
       <c r="G33" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="I33" s="2" t="s">
-        <v>227</v>
+        <v>30</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>222</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>65</v>
+        <v>196</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2652,108 +2608,24 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="2" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>228</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="N34" s="1">
-        <v>1.49</v>
+        <v>0.4012</v>
       </c>
       <c r="O34" s="1">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="1">
-        <v>1</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="N36" s="1">
-        <v>0.4012</v>
-      </c>
-      <c r="O36" s="1">
         <v>0.4012</v>
       </c>
     </row>

</xml_diff>